<commit_message>
Adding test data and settings
</commit_message>
<xml_diff>
--- a/Test Data/Dummy Contacts.xlsx
+++ b/Test Data/Dummy Contacts.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27717"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2CA5F44-FBF0-4AAE-95F6-FE6673698C49}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew_Howes\Repos\XTBPlugins.DataImport\Test Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018A44D7-1ADD-470E-83E1-ED07CA6DD839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="1812" windowWidth="14400" windowHeight="7272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,10 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-  </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,13 +155,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,22 +496,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -562,7 +563,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -588,7 +589,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -613,9 +614,6 @@
       <c r="H4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="I6" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adding to Developing.md to make it more clear. Adding new test columns for latest release.
</commit_message>
<xml_diff>
--- a/Test Data/Dummy Contacts.xlsx
+++ b/Test Data/Dummy Contacts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew_Howes\Repos\XTBPlugins.DataImport\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD1739F-0ADD-4B39-9B43-A82F7EBC0FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C8E043-F257-4499-AE18-DE9B8B7021EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="96" yWindow="216" windowWidth="22944" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>First Name</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Saun</t>
   </si>
   <si>
-    <t>andy@andyhowes.co</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -153,6 +150,24 @@
   </si>
   <si>
     <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Statuscode</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>ShouldFail</t>
+  </si>
+  <si>
+    <t>Sammmy.sean@samsam.com</t>
   </si>
 </sst>
 </file>
@@ -544,22 +559,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="40.90625" customWidth="1"/>
-    <col min="7" max="7" width="19.36328125" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="40.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,22 +591,25 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -599,7 +617,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1">
         <v>123456789</v>
@@ -608,30 +626,33 @@
         <v>36522</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>85462578</v>
@@ -640,30 +661,33 @@
         <v>23350</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>58468547</v>
@@ -672,19 +696,22 @@
         <v>29225</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -692,7 +719,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1">
         <v>123456789</v>
@@ -701,27 +728,30 @@
         <v>36522</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1">
         <v>85462578</v>
@@ -730,30 +760,33 @@
         <v>23350</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1">
         <v>58468547</v>
@@ -762,22 +795,25 @@
         <v>29225</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -785,7 +821,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1">
         <v>123456789</v>
@@ -794,27 +830,30 @@
         <v>36522</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1">
         <v>85462578</v>
@@ -823,30 +862,33 @@
         <v>23350</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="K9" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1">
         <v>58468547</v>
@@ -855,19 +897,22 @@
         <v>29225</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J10" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="K10" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>